<commit_message>
Added example showing the alternative template options
</commit_message>
<xml_diff>
--- a/examples/demo_marks.xlsx
+++ b/examples/demo_marks.xlsx
@@ -12,7 +12,7 @@
     <sheet name="marks" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">marks!$B$2:$AV$11</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">marks!$B$2:$AV$6</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">participants!$A$2:$F$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="40">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t xml:space="preserve">wonderwoman@noboysallowed.aol.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barrya@ccpd.gov</t>
   </si>
   <si>
     <t xml:space="preserve">comments</t>
@@ -124,13 +133,10 @@
 8%</t>
   </si>
   <si>
-    <t xml:space="preserve">Bumped 1.2 to 4 from 3.5 to get overall to 80</t>
+    <t xml:space="preserve">Bumped 1.2 to 4 from 3.5</t>
   </si>
   <si>
     <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes, extension, very late</t>
   </si>
   <si>
     <t xml:space="preserve">fine
@@ -138,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">no report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extension, very late</t>
   </si>
 </sst>
 </file>
@@ -217,7 +226,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,12 +251,6 @@
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -283,7 +286,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -360,7 +363,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,7 +384,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -392,12 +395,16 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -563,7 +570,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFC000"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -594,13 +601,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ5"/>
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.35546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -763,9 +770,35 @@
       <c r="L5" s="2"/>
       <c r="M5" s="11"/>
     </row>
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1234569</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <f aca="false">SUM(H6*H$1+I6*I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <f aca="false">INDEX(marks!F:F,MATCH(C6,marks!B:B,0))</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="12"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:F5"/>
-  <conditionalFormatting sqref="G3:G5">
+  <conditionalFormatting sqref="G3:G6">
     <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>50</formula>
     </cfRule>
@@ -774,6 +807,7 @@
     <hyperlink ref="E3" r:id="rId1" display="batman@wayneenterprises.com"/>
     <hyperlink ref="E4" r:id="rId2" display="superman@dailyplanet.com"/>
     <hyperlink ref="E5" r:id="rId3" display="wonderwoman@noboysallowed.aol.com"/>
+    <hyperlink ref="E6" r:id="rId4" display="barrya@ccpd.gov"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -782,7 +816,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -794,16 +828,17 @@
   <dimension ref="A1:AV1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C424" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q5" activeCellId="0" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="A424" activeCellId="0" sqref="A424"/>
+      <selection pane="bottomRight" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.35546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="10.5"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.25"/>
@@ -870,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="AE1" s="14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AF1" s="14"/>
       <c r="AG1" s="14"/>
@@ -892,43 +927,43 @@
     </row>
     <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2" s="15" t="str">
         <f aca="false">CHAR(10)&amp;"submitted"</f>
         <v>submitted</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2" s="16" t="str">
         <f aca="false">CHAR(10)&amp;"%"</f>
         <v>%</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K2" s="15" t="str">
         <f aca="false">CHAR(10)&amp;"total"</f>
         <v>total</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M2" s="17" t="n">
         <v>1.1</v>
@@ -982,7 +1017,7 @@
         <v>4</v>
       </c>
       <c r="AD2" s="17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AE2" s="18" t="n">
         <v>1.1</v>
@@ -1036,7 +1071,7 @@
         <v>4</v>
       </c>
       <c r="AV2" s="18" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1048,10 +1083,10 @@
         <v>1234566</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E3" s="21" t="str">
         <f aca="false">IF(LEN( AE3)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF3)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG3)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH3)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI3)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ3)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK3)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL3)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM3)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN3)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO3)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP3)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ3)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR3)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS3)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT3)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU3)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV3)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV3&amp;CHAR(10),"")</f>
@@ -1117,7 +1152,7 @@
         <v>37</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M3" s="7" t="n">
         <v>3</v>
@@ -1174,58 +1209,58 @@
         <v>6</v>
       </c>
       <c r="AE3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AF3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AG3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AH3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AI3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AJ3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AK3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AL3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AM3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AN3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AO3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AP3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AQ3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AR3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AS3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AT3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AU3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AV3" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1237,10 +1272,10 @@
         <v>1234567</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E4" s="21" t="str">
         <f aca="false">IF(LEN( AE4)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF4)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG4)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH4)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI4)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ4)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK4)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL4)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM4)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN4)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO4)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP4)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ4)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR4)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS4)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT4)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU4)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV4)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV4&amp;CHAR(10),"")</f>
@@ -1361,58 +1396,58 @@
         <v>6</v>
       </c>
       <c r="AE4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AF4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AG4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AH4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AI4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AJ4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AK4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AL4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AM4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AN4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AO4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AP4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AQ4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AR4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AS4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AT4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AU4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AV4" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1424,10 +1459,10 @@
         <v>1234568</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" s="21" t="str">
         <f aca="false">IF(LEN( AE5)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF5)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG5)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH5)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI5)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ5)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK5)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL5)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM5)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN5)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO5)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP5)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ5)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR5)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS5)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT5)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU5)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV5)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV5&amp;CHAR(10),"")</f>
@@ -1548,271 +1583,544 @@
         <v>7</v>
       </c>
       <c r="AE5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AF5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AG5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AH5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AI5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AJ5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AK5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AL5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AM5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AN5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AO5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AP5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AQ5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AR5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AS5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AT5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AU5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AV5" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="str">
+        <f aca="false">INDEX(participants!A:A,MATCH(B6,participants!C:C,0))&amp;" "&amp;INDEX(participants!B:B,MATCH(B6,participants!C:C,0))</f>
+        <v>Barry Alan</v>
+      </c>
+      <c r="B6" s="28" t="n">
+        <v>1234569</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>39</v>
+      </c>
       <c r="D6" s="19"/>
-      <c r="E6" s="19" t="str">
-        <f aca="false">IF(LEN(M6)&gt;0,"## "&amp;M$2&amp;CHAR(10)&amp;CHAR(10)&amp;M6&amp;CHAR(10),"")&amp; IF(LEN(N6)&gt;0,"## "&amp;N$2&amp;CHAR(10)&amp;CHAR(10)&amp;N6&amp;CHAR(10),"")&amp; IF(LEN(O6)&gt;0,"## "&amp;O$2&amp;CHAR(10)&amp;CHAR(10)&amp;O6&amp;CHAR(10),"")&amp; IF(LEN(P6)&gt;0,"## "&amp;P$2&amp;CHAR(10)&amp;CHAR(10)&amp;P6&amp;CHAR(10),"")&amp; IF(LEN(Q6)&gt;0,"## "&amp;Q$2&amp;CHAR(10)&amp;CHAR(10)&amp;Q6&amp;CHAR(10),"")&amp; IF(LEN(R6)&gt;0,"## "&amp;R$2&amp;CHAR(10)&amp;CHAR(10)&amp;R6&amp;CHAR(10),"")&amp; IF(LEN(S6)&gt;0,"## "&amp;S$2&amp;CHAR(10)&amp;CHAR(10)&amp;S6&amp;CHAR(10),"")&amp; IF(LEN(T6)&gt;0,"## "&amp;T$2&amp;CHAR(10)&amp;CHAR(10)&amp;T6&amp;CHAR(10),"")&amp; IF(LEN(U6)&gt;0,"## "&amp;U$2&amp;CHAR(10)&amp;CHAR(10)&amp;U6&amp;CHAR(10),"")&amp; IF(LEN(V6)&gt;0,"## "&amp;V$2&amp;CHAR(10)&amp;CHAR(10)&amp;V6&amp;CHAR(10),"")&amp; IF(LEN(W6)&gt;0,"## "&amp;W$2&amp;CHAR(10)&amp;CHAR(10)&amp;W6&amp;CHAR(10),"")&amp; IF(LEN(X6)&gt;0,"## "&amp;X$2&amp;CHAR(10)&amp;CHAR(10)&amp;X6&amp;CHAR(10),"")&amp; IF(LEN(Y6)&gt;0,"## "&amp;Y$2&amp;CHAR(10)&amp;CHAR(10)&amp;Y6&amp;CHAR(10),"")&amp; IF(LEN(Z6)&gt;0,"## "&amp;Z$2&amp;CHAR(10)&amp;CHAR(10)&amp;Z6&amp;CHAR(10),"")&amp; IF(LEN(AA6)&gt;0,"## "&amp;AA$2&amp;CHAR(10)&amp;CHAR(10)&amp;AA6&amp;CHAR(10),"")&amp; IF(LEN(AB6)&gt;0,"## "&amp;AB$2&amp;CHAR(10)&amp;CHAR(10)&amp;AB6&amp;CHAR(10),"")&amp; IF(LEN(AC6)&gt;0,"## "&amp;AC$2&amp;CHAR(10)&amp;CHAR(10)&amp;AC6&amp;CHAR(10),"")&amp; IF(LEN(AD6)&gt;0,"## "&amp;AD$2&amp;CHAR(10)&amp;CHAR(10)&amp;AD6&amp;CHAR(10),"")</f>
+      <c r="E6" s="21" t="str">
+        <f aca="false">IF(LEN( AE6)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF6)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG6)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH6)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI6)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ6)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK6)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL6)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM6)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN6)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO6)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP6)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ6)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR6)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS6)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT6)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU6)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV6)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV6&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="F6" s="22" t="n">
+        <f aca="false">ROUND(K6/70*100,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="22" t="n">
+        <f aca="false">ROUND(SUM(M6:P6)/SUM(M$1:P$1)*100,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="22" t="n">
+        <f aca="false">ROUND(SUM(N6:Q6)/SUM(N$1:Q$1)*100,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="22" t="n">
+        <f aca="false">ROUND(SUM(O6:R6)/SUM(O$1:R$1)*100,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="22" t="n">
+        <f aca="false">ROUND(SUM(P6:S6)/SUM(P$1:S$1)*100,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="22" t="n">
+        <f aca="false">ROUNDUP(SUM(M6:AD6),0)</f>
+        <v>0</v>
+      </c>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19" t="str">
-        <f aca="false">IF(LEN(M7)&gt;0,"## "&amp;M$2&amp;CHAR(10)&amp;CHAR(10)&amp;M7&amp;CHAR(10),"")&amp; IF(LEN(N7)&gt;0,"## "&amp;N$2&amp;CHAR(10)&amp;CHAR(10)&amp;N7&amp;CHAR(10),"")&amp; IF(LEN(O7)&gt;0,"## "&amp;O$2&amp;CHAR(10)&amp;CHAR(10)&amp;O7&amp;CHAR(10),"")&amp; IF(LEN(P7)&gt;0,"## "&amp;P$2&amp;CHAR(10)&amp;CHAR(10)&amp;P7&amp;CHAR(10),"")&amp; IF(LEN(Q7)&gt;0,"## "&amp;Q$2&amp;CHAR(10)&amp;CHAR(10)&amp;Q7&amp;CHAR(10),"")&amp; IF(LEN(R7)&gt;0,"## "&amp;R$2&amp;CHAR(10)&amp;CHAR(10)&amp;R7&amp;CHAR(10),"")&amp; IF(LEN(S7)&gt;0,"## "&amp;S$2&amp;CHAR(10)&amp;CHAR(10)&amp;S7&amp;CHAR(10),"")&amp; IF(LEN(T7)&gt;0,"## "&amp;T$2&amp;CHAR(10)&amp;CHAR(10)&amp;T7&amp;CHAR(10),"")&amp; IF(LEN(U7)&gt;0,"## "&amp;U$2&amp;CHAR(10)&amp;CHAR(10)&amp;U7&amp;CHAR(10),"")&amp; IF(LEN(V7)&gt;0,"## "&amp;V$2&amp;CHAR(10)&amp;CHAR(10)&amp;V7&amp;CHAR(10),"")&amp; IF(LEN(W7)&gt;0,"## "&amp;W$2&amp;CHAR(10)&amp;CHAR(10)&amp;W7&amp;CHAR(10),"")&amp; IF(LEN(X7)&gt;0,"## "&amp;X$2&amp;CHAR(10)&amp;CHAR(10)&amp;X7&amp;CHAR(10),"")&amp; IF(LEN(Y7)&gt;0,"## "&amp;Y$2&amp;CHAR(10)&amp;CHAR(10)&amp;Y7&amp;CHAR(10),"")&amp; IF(LEN(Z7)&gt;0,"## "&amp;Z$2&amp;CHAR(10)&amp;CHAR(10)&amp;Z7&amp;CHAR(10),"")&amp; IF(LEN(AA7)&gt;0,"## "&amp;AA$2&amp;CHAR(10)&amp;CHAR(10)&amp;AA7&amp;CHAR(10),"")&amp; IF(LEN(AB7)&gt;0,"## "&amp;AB$2&amp;CHAR(10)&amp;CHAR(10)&amp;AB7&amp;CHAR(10),"")&amp; IF(LEN(AC7)&gt;0,"## "&amp;AC$2&amp;CHAR(10)&amp;CHAR(10)&amp;AC7&amp;CHAR(10),"")&amp; IF(LEN(AD7)&gt;0,"## "&amp;AD$2&amp;CHAR(10)&amp;CHAR(10)&amp;AD7&amp;CHAR(10),"")</f>
-        <v/>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="str">
-        <f aca="false">IF(LEN(M8)&gt;0,"## "&amp;M$2&amp;CHAR(10)&amp;CHAR(10)&amp;M8&amp;CHAR(10),"")&amp; IF(LEN(N8)&gt;0,"## "&amp;N$2&amp;CHAR(10)&amp;CHAR(10)&amp;N8&amp;CHAR(10),"")&amp; IF(LEN(O8)&gt;0,"## "&amp;O$2&amp;CHAR(10)&amp;CHAR(10)&amp;O8&amp;CHAR(10),"")&amp; IF(LEN(P8)&gt;0,"## "&amp;P$2&amp;CHAR(10)&amp;CHAR(10)&amp;P8&amp;CHAR(10),"")&amp; IF(LEN(Q8)&gt;0,"## "&amp;Q$2&amp;CHAR(10)&amp;CHAR(10)&amp;Q8&amp;CHAR(10),"")&amp; IF(LEN(R8)&gt;0,"## "&amp;R$2&amp;CHAR(10)&amp;CHAR(10)&amp;R8&amp;CHAR(10),"")&amp; IF(LEN(S8)&gt;0,"## "&amp;S$2&amp;CHAR(10)&amp;CHAR(10)&amp;S8&amp;CHAR(10),"")&amp; IF(LEN(T8)&gt;0,"## "&amp;T$2&amp;CHAR(10)&amp;CHAR(10)&amp;T8&amp;CHAR(10),"")&amp; IF(LEN(U8)&gt;0,"## "&amp;U$2&amp;CHAR(10)&amp;CHAR(10)&amp;U8&amp;CHAR(10),"")&amp; IF(LEN(V8)&gt;0,"## "&amp;V$2&amp;CHAR(10)&amp;CHAR(10)&amp;V8&amp;CHAR(10),"")&amp; IF(LEN(W8)&gt;0,"## "&amp;W$2&amp;CHAR(10)&amp;CHAR(10)&amp;W8&amp;CHAR(10),"")&amp; IF(LEN(X8)&gt;0,"## "&amp;X$2&amp;CHAR(10)&amp;CHAR(10)&amp;X8&amp;CHAR(10),"")&amp; IF(LEN(Y8)&gt;0,"## "&amp;Y$2&amp;CHAR(10)&amp;CHAR(10)&amp;Y8&amp;CHAR(10),"")&amp; IF(LEN(Z8)&gt;0,"## "&amp;Z$2&amp;CHAR(10)&amp;CHAR(10)&amp;Z8&amp;CHAR(10),"")&amp; IF(LEN(AA8)&gt;0,"## "&amp;AA$2&amp;CHAR(10)&amp;CHAR(10)&amp;AA8&amp;CHAR(10),"")&amp; IF(LEN(AB8)&gt;0,"## "&amp;AB$2&amp;CHAR(10)&amp;CHAR(10)&amp;AB8&amp;CHAR(10),"")&amp; IF(LEN(AC8)&gt;0,"## "&amp;AC$2&amp;CHAR(10)&amp;CHAR(10)&amp;AC8&amp;CHAR(10),"")&amp; IF(LEN(AD8)&gt;0,"## "&amp;AD$2&amp;CHAR(10)&amp;CHAR(10)&amp;AD8&amp;CHAR(10),"")</f>
-        <v/>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19" t="str">
-        <f aca="false">IF(LEN(M9)&gt;0,"## "&amp;M$2&amp;CHAR(10)&amp;CHAR(10)&amp;M9&amp;CHAR(10),"")&amp; IF(LEN(N9)&gt;0,"## "&amp;N$2&amp;CHAR(10)&amp;CHAR(10)&amp;N9&amp;CHAR(10),"")&amp; IF(LEN(O9)&gt;0,"## "&amp;O$2&amp;CHAR(10)&amp;CHAR(10)&amp;O9&amp;CHAR(10),"")&amp; IF(LEN(P9)&gt;0,"## "&amp;P$2&amp;CHAR(10)&amp;CHAR(10)&amp;P9&amp;CHAR(10),"")&amp; IF(LEN(Q9)&gt;0,"## "&amp;Q$2&amp;CHAR(10)&amp;CHAR(10)&amp;Q9&amp;CHAR(10),"")&amp; IF(LEN(R9)&gt;0,"## "&amp;R$2&amp;CHAR(10)&amp;CHAR(10)&amp;R9&amp;CHAR(10),"")&amp; IF(LEN(S9)&gt;0,"## "&amp;S$2&amp;CHAR(10)&amp;CHAR(10)&amp;S9&amp;CHAR(10),"")&amp; IF(LEN(T9)&gt;0,"## "&amp;T$2&amp;CHAR(10)&amp;CHAR(10)&amp;T9&amp;CHAR(10),"")&amp; IF(LEN(U9)&gt;0,"## "&amp;U$2&amp;CHAR(10)&amp;CHAR(10)&amp;U9&amp;CHAR(10),"")&amp; IF(LEN(V9)&gt;0,"## "&amp;V$2&amp;CHAR(10)&amp;CHAR(10)&amp;V9&amp;CHAR(10),"")&amp; IF(LEN(W9)&gt;0,"## "&amp;W$2&amp;CHAR(10)&amp;CHAR(10)&amp;W9&amp;CHAR(10),"")&amp; IF(LEN(X9)&gt;0,"## "&amp;X$2&amp;CHAR(10)&amp;CHAR(10)&amp;X9&amp;CHAR(10),"")&amp; IF(LEN(Y9)&gt;0,"## "&amp;Y$2&amp;CHAR(10)&amp;CHAR(10)&amp;Y9&amp;CHAR(10),"")&amp; IF(LEN(Z9)&gt;0,"## "&amp;Z$2&amp;CHAR(10)&amp;CHAR(10)&amp;Z9&amp;CHAR(10),"")&amp; IF(LEN(AA9)&gt;0,"## "&amp;AA$2&amp;CHAR(10)&amp;CHAR(10)&amp;AA9&amp;CHAR(10),"")&amp; IF(LEN(AB9)&gt;0,"## "&amp;AB$2&amp;CHAR(10)&amp;CHAR(10)&amp;AB9&amp;CHAR(10),"")&amp; IF(LEN(AC9)&gt;0,"## "&amp;AC$2&amp;CHAR(10)&amp;CHAR(10)&amp;AC9&amp;CHAR(10),"")&amp; IF(LEN(AD9)&gt;0,"## "&amp;AD$2&amp;CHAR(10)&amp;CHAR(10)&amp;AD9&amp;CHAR(10),"")</f>
-        <v/>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19" t="str">
-        <f aca="false">IF(LEN(M10)&gt;0,"## "&amp;M$2&amp;CHAR(10)&amp;CHAR(10)&amp;M10&amp;CHAR(10),"")&amp; IF(LEN(N10)&gt;0,"## "&amp;N$2&amp;CHAR(10)&amp;CHAR(10)&amp;N10&amp;CHAR(10),"")&amp; IF(LEN(O10)&gt;0,"## "&amp;O$2&amp;CHAR(10)&amp;CHAR(10)&amp;O10&amp;CHAR(10),"")&amp; IF(LEN(P10)&gt;0,"## "&amp;P$2&amp;CHAR(10)&amp;CHAR(10)&amp;P10&amp;CHAR(10),"")&amp; IF(LEN(Q10)&gt;0,"## "&amp;Q$2&amp;CHAR(10)&amp;CHAR(10)&amp;Q10&amp;CHAR(10),"")&amp; IF(LEN(R10)&gt;0,"## "&amp;R$2&amp;CHAR(10)&amp;CHAR(10)&amp;R10&amp;CHAR(10),"")&amp; IF(LEN(S10)&gt;0,"## "&amp;S$2&amp;CHAR(10)&amp;CHAR(10)&amp;S10&amp;CHAR(10),"")&amp; IF(LEN(T10)&gt;0,"## "&amp;T$2&amp;CHAR(10)&amp;CHAR(10)&amp;T10&amp;CHAR(10),"")&amp; IF(LEN(U10)&gt;0,"## "&amp;U$2&amp;CHAR(10)&amp;CHAR(10)&amp;U10&amp;CHAR(10),"")&amp; IF(LEN(V10)&gt;0,"## "&amp;V$2&amp;CHAR(10)&amp;CHAR(10)&amp;V10&amp;CHAR(10),"")&amp; IF(LEN(W10)&gt;0,"## "&amp;W$2&amp;CHAR(10)&amp;CHAR(10)&amp;W10&amp;CHAR(10),"")&amp; IF(LEN(X10)&gt;0,"## "&amp;X$2&amp;CHAR(10)&amp;CHAR(10)&amp;X10&amp;CHAR(10),"")&amp; IF(LEN(Y10)&gt;0,"## "&amp;Y$2&amp;CHAR(10)&amp;CHAR(10)&amp;Y10&amp;CHAR(10),"")&amp; IF(LEN(Z10)&gt;0,"## "&amp;Z$2&amp;CHAR(10)&amp;CHAR(10)&amp;Z10&amp;CHAR(10),"")&amp; IF(LEN(AA10)&gt;0,"## "&amp;AA$2&amp;CHAR(10)&amp;CHAR(10)&amp;AA10&amp;CHAR(10),"")&amp; IF(LEN(AB10)&gt;0,"## "&amp;AB$2&amp;CHAR(10)&amp;CHAR(10)&amp;AB10&amp;CHAR(10),"")&amp; IF(LEN(AC10)&gt;0,"## "&amp;AC$2&amp;CHAR(10)&amp;CHAR(10)&amp;AC10&amp;CHAR(10),"")&amp; IF(LEN(AD10)&gt;0,"## "&amp;AD$2&amp;CHAR(10)&amp;CHAR(10)&amp;AD10&amp;CHAR(10),"")</f>
-        <v/>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="19"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="19"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="19"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="19"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="19"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="19"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="19"/>
-    </row>
+    <row r="1048126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048127" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048128" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048129" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048130" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048131" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048132" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048133" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048134" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048135" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048136" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048137" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048138" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048139" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048140" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048141" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048142" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048143" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048144" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048145" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048146" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048147" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048148" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048149" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048150" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048151" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048152" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048153" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048154" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048155" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048156" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048157" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048158" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048159" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048160" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048161" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048162" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048163" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048164" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048165" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048166" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048167" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048168" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048169" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048170" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048171" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048172" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048173" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048174" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048175" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048176" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048177" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048178" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048179" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048180" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048181" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048182" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048183" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048184" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048185" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048186" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048187" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048188" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048189" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048190" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048191" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048192" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048193" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048194" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048195" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048196" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048197" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048198" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048199" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048200" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048201" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048202" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048203" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048204" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048205" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048206" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048207" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048208" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048209" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048210" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048211" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048212" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048213" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048214" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048215" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048216" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048217" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048218" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048219" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048220" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048221" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048222" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048223" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048224" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048225" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048226" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048227" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048228" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048229" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048230" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048231" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048232" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048233" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048234" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048235" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048236" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048237" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048238" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048239" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048240" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048241" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048242" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048243" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048244" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048245" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048246" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048247" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048248" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048249" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048250" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048251" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048252" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048253" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048254" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048255" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048256" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048257" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048258" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048259" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048260" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048261" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048262" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048264" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048265" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048266" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048267" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048268" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048269" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048270" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048271" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048272" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048273" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048274" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048275" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048276" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048277" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048278" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048279" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048280" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048281" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048282" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048283" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048284" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048285" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048286" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048287" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048288" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048289" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048290" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048291" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048292" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048293" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048294" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048295" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048296" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048297" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048298" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048299" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048300" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048301" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048302" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048303" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048304" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048305" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048306" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048307" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048308" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048309" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048310" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048311" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048312" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048313" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048314" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048315" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048316" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048317" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048318" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048319" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048320" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048321" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048322" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048323" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048324" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048325" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048326" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048327" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048328" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048329" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048330" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048331" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048332" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048333" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048334" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048335" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048336" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048337" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048338" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048339" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048340" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048341" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048342" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048343" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048344" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048345" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048346" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048347" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048348" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048349" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048350" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048351" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048352" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048353" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048354" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048355" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048356" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048357" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048358" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048359" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048360" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048361" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048421" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048422" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048426" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048427" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048428" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1823,7 +2131,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="B2:AV11"/>
+  <autoFilter ref="B2:AV6"/>
   <mergeCells count="1">
     <mergeCell ref="AE1:AV1"/>
   </mergeCells>
@@ -1837,7 +2145,7 @@
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K999991">
+  <conditionalFormatting sqref="K3:K999549">
     <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>70</formula>
     </cfRule>

</xml_diff>

<commit_message>
Improved documentation and explanation of example.
Added explanatory text to script and template
</commit_message>
<xml_diff>
--- a/examples/demo_marks.xlsx
+++ b/examples/demo_marks.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="participants" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="marks" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="participants" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="marks" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">marks!$B$2:$AV$6</definedName>
@@ -291,119 +291,119 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,7 +420,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -428,7 +428,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -450,6 +450,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF999999"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -457,6 +458,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -464,6 +466,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -471,6 +474,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFDDE8CB"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -478,6 +482,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFDEE6EF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -596,8 +601,114 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -607,194 +718,194 @@
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="7.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="33.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G1" s="4"/>
-      <c r="H1" s="3" t="n">
+    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="5"/>
+      <c r="H1" s="4" t="n">
         <v>0.7</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="4" t="n">
         <v>0.3</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="AMJ1" s="0"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="AMJ1" s="1"/>
     </row>
-    <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="AMJ2" s="0"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="AMJ2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="8" t="n">
         <v>1234566</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="10" t="n">
         <f aca="false">SUM(H3*H$1+I3*I$1)</f>
         <v>58.1</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="9" t="n">
         <f aca="false">INDEX(marks!F:F,MATCH(C3,marks!B:B,0))</f>
         <v>53</v>
       </c>
-      <c r="I3" s="8" t="n">
+      <c r="I3" s="9" t="n">
         <v>70</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="8" t="n">
         <v>1234567</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="9" t="n">
+      <c r="G4" s="10" t="n">
         <f aca="false">SUM(H4*H$1+I4*I$1)</f>
         <v>49.1</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="H4" s="9" t="n">
         <f aca="false">INDEX(marks!F:F,MATCH(C4,marks!B:B,0))</f>
         <v>53</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="I4" s="9" t="n">
         <v>40</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <v>1234568</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <f aca="false">SUM(H5*H$1+I5*I$1)</f>
         <v>61.9</v>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="9" t="n">
         <f aca="false">INDEX(marks!F:F,MATCH(C5,marks!B:B,0))</f>
         <v>67</v>
       </c>
-      <c r="I5" s="8" t="n">
+      <c r="I5" s="9" t="n">
         <v>50</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="12"/>
     </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="17.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>1234569</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="10" t="n">
         <f aca="false">SUM(H6*H$1+I6*I$1)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="9" t="n">
         <f aca="false">INDEX(marks!F:F,MATCH(C6,marks!B:B,0))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="12"/>
+      <c r="I6" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:F5"/>
@@ -821,274 +932,274 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AV1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C424" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A424" activeCellId="0" sqref="A424"/>
-      <selection pane="bottomRight" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="10.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="10.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="0" width="4.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="13" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="5.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="31" style="0" width="3.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="10.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="1" width="4.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="13" style="1" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="5.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="31" style="1" width="3.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="M1" s="13" t="n">
+      <c r="M1" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="N1" s="13" t="n">
+      <c r="N1" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="O1" s="13" t="n">
+      <c r="O1" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="P1" s="13" t="n">
+      <c r="P1" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="Q1" s="13" t="n">
+      <c r="Q1" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="R1" s="13" t="n">
+      <c r="R1" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="S1" s="13" t="n">
+      <c r="S1" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="T1" s="13" t="n">
+      <c r="T1" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="U1" s="13" t="n">
+      <c r="U1" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="V1" s="13" t="n">
+      <c r="V1" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="W1" s="13" t="n">
+      <c r="W1" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="X1" s="13" t="n">
+      <c r="X1" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="Y1" s="13" t="n">
+      <c r="Y1" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="Z1" s="13" t="n">
+      <c r="Z1" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="AA1" s="13" t="n">
+      <c r="AA1" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="AB1" s="13" t="n">
+      <c r="AB1" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="AC1" s="13" t="n">
+      <c r="AC1" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="AD1" s="13" t="n">
+      <c r="AD1" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AE1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-      <c r="AJ1" s="14"/>
-      <c r="AK1" s="14"/>
-      <c r="AL1" s="14"/>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
-      <c r="AO1" s="14"/>
-      <c r="AP1" s="14"/>
-      <c r="AQ1" s="14"/>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
     </row>
-    <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+    <row r="2" customFormat="false" ht="48.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="15" t="str">
+      <c r="C2" s="16" t="str">
         <f aca="false">CHAR(10)&amp;"submitted"</f>
         <v>submitted</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="16" t="str">
+      <c r="F2" s="17" t="str">
         <f aca="false">CHAR(10)&amp;"%"</f>
         <v>%</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="15" t="str">
+      <c r="K2" s="16" t="str">
         <f aca="false">CHAR(10)&amp;"total"</f>
         <v>total</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="17" t="n">
+      <c r="M2" s="18" t="n">
         <v>1.1</v>
       </c>
-      <c r="N2" s="17" t="n">
+      <c r="N2" s="18" t="n">
         <v>1.2</v>
       </c>
-      <c r="O2" s="17" t="n">
+      <c r="O2" s="18" t="n">
         <v>1.3</v>
       </c>
-      <c r="P2" s="17" t="n">
+      <c r="P2" s="18" t="n">
         <v>1.4</v>
       </c>
-      <c r="Q2" s="17" t="n">
+      <c r="Q2" s="18" t="n">
         <v>1.5</v>
       </c>
-      <c r="R2" s="17" t="n">
+      <c r="R2" s="18" t="n">
         <v>1.6</v>
       </c>
-      <c r="S2" s="17" t="n">
+      <c r="S2" s="18" t="n">
         <v>1.7</v>
       </c>
-      <c r="T2" s="17" t="n">
+      <c r="T2" s="18" t="n">
         <v>1.8</v>
       </c>
-      <c r="U2" s="17" t="n">
+      <c r="U2" s="18" t="n">
         <v>1.9</v>
       </c>
-      <c r="V2" s="17" t="n">
+      <c r="V2" s="18" t="n">
         <v>2.1</v>
       </c>
-      <c r="W2" s="17" t="n">
+      <c r="W2" s="18" t="n">
         <v>2.2</v>
       </c>
-      <c r="X2" s="17" t="n">
+      <c r="X2" s="18" t="n">
         <v>2.3</v>
       </c>
-      <c r="Y2" s="17" t="n">
+      <c r="Y2" s="18" t="n">
         <v>2.4</v>
       </c>
-      <c r="Z2" s="17" t="n">
+      <c r="Z2" s="18" t="n">
         <v>2.5</v>
       </c>
-      <c r="AA2" s="17" t="n">
+      <c r="AA2" s="18" t="n">
         <v>3.1</v>
       </c>
-      <c r="AB2" s="17" t="n">
+      <c r="AB2" s="18" t="n">
         <v>3.2</v>
       </c>
-      <c r="AC2" s="17" t="n">
+      <c r="AC2" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="AD2" s="17" t="s">
+      <c r="AD2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="18" t="n">
+      <c r="AE2" s="19" t="n">
         <v>1.1</v>
       </c>
-      <c r="AF2" s="18" t="n">
+      <c r="AF2" s="19" t="n">
         <v>1.2</v>
       </c>
-      <c r="AG2" s="18" t="n">
+      <c r="AG2" s="19" t="n">
         <v>1.3</v>
       </c>
-      <c r="AH2" s="18" t="n">
+      <c r="AH2" s="19" t="n">
         <v>1.4</v>
       </c>
-      <c r="AI2" s="18" t="n">
+      <c r="AI2" s="19" t="n">
         <v>1.5</v>
       </c>
-      <c r="AJ2" s="18" t="n">
+      <c r="AJ2" s="19" t="n">
         <v>1.6</v>
       </c>
-      <c r="AK2" s="18" t="n">
+      <c r="AK2" s="19" t="n">
         <v>1.7</v>
       </c>
-      <c r="AL2" s="18" t="n">
+      <c r="AL2" s="19" t="n">
         <v>1.8</v>
       </c>
-      <c r="AM2" s="18" t="n">
+      <c r="AM2" s="19" t="n">
         <v>1.9</v>
       </c>
-      <c r="AN2" s="18" t="n">
+      <c r="AN2" s="19" t="n">
         <v>2.1</v>
       </c>
-      <c r="AO2" s="18" t="n">
+      <c r="AO2" s="19" t="n">
         <v>2.2</v>
       </c>
-      <c r="AP2" s="18" t="n">
+      <c r="AP2" s="19" t="n">
         <v>2.3</v>
       </c>
-      <c r="AQ2" s="18" t="n">
+      <c r="AQ2" s="19" t="n">
         <v>2.4</v>
       </c>
-      <c r="AR2" s="18" t="n">
+      <c r="AR2" s="19" t="n">
         <v>2.5</v>
       </c>
-      <c r="AS2" s="18" t="n">
+      <c r="AS2" s="19" t="n">
         <v>3.1</v>
       </c>
-      <c r="AT2" s="18" t="n">
+      <c r="AT2" s="19" t="n">
         <v>3.2</v>
       </c>
-      <c r="AU2" s="18" t="n">
+      <c r="AU2" s="19" t="n">
         <v>4</v>
       </c>
-      <c r="AV2" s="18" t="s">
+      <c r="AV2" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="str">
+      <c r="A3" s="20" t="str">
         <f aca="false">INDEX(participants!A:A,MATCH(B3,participants!C:C,0))&amp;" "&amp;INDEX(participants!B:B,MATCH(B3,participants!C:C,0))</f>
         <v>Bruce Wayne</v>
       </c>
-      <c r="B3" s="19" t="n">
+      <c r="B3" s="20" t="n">
         <v>1234566</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="21" t="str">
+      <c r="E3" s="22" t="str">
         <f aca="false">IF(LEN( AE3)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF3)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG3)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH3)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI3)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ3)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK3)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL3)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM3)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN3)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO3)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP3)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ3)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR3)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS3)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT3)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU3)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU3&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV3)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV3&amp;CHAR(10),"")</f>
         <v>## 1.1
 Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat
@@ -1127,157 +1238,157 @@
 ## Presentation
 Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat</v>
       </c>
-      <c r="F3" s="22" t="n">
+      <c r="F3" s="23" t="n">
         <f aca="false">ROUND(K3/70*100,0)</f>
         <v>53</v>
       </c>
-      <c r="G3" s="22" t="n">
+      <c r="G3" s="23" t="n">
         <f aca="false">ROUND(SUM(M3:P3)/SUM(M$1:P$1)*100,0)</f>
         <v>77</v>
       </c>
-      <c r="H3" s="22" t="n">
+      <c r="H3" s="23" t="n">
         <f aca="false">ROUND(SUM(N3:Q3)/SUM(N$1:Q$1)*100,0)</f>
         <v>50</v>
       </c>
-      <c r="I3" s="22" t="n">
+      <c r="I3" s="23" t="n">
         <f aca="false">ROUND(SUM(O3:R3)/SUM(O$1:R$1)*100,0)</f>
         <v>32</v>
       </c>
-      <c r="J3" s="22" t="n">
+      <c r="J3" s="23" t="n">
         <f aca="false">ROUND(SUM(P3:S3)/SUM(P$1:S$1)*100,0)</f>
         <v>16</v>
       </c>
-      <c r="K3" s="22" t="n">
+      <c r="K3" s="23" t="n">
         <f aca="false">ROUNDUP(SUM(M3:AD3),0)</f>
         <v>37</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="7" t="n">
+      <c r="M3" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N3" s="7" t="n">
+      <c r="N3" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="O3" s="7" t="n">
+      <c r="O3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="P3" s="7" t="n">
+      <c r="P3" s="8" t="n">
         <v>2.5</v>
       </c>
-      <c r="Q3" s="7" t="n">
+      <c r="Q3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="R3" s="7" t="n">
+      <c r="R3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="S3" s="7" t="n">
+      <c r="S3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="T3" s="7" t="n">
+      <c r="T3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="U3" s="7" t="n">
+      <c r="U3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="V3" s="7" t="n">
+      <c r="V3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="W3" s="7" t="n">
+      <c r="W3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="X3" s="7" t="n">
+      <c r="X3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="Y3" s="7" t="n">
+      <c r="Y3" s="8" t="n">
         <v>2.5</v>
       </c>
-      <c r="Z3" s="7" t="n">
+      <c r="Z3" s="8" t="n">
         <v>2.5</v>
       </c>
-      <c r="AA3" s="7" t="n">
+      <c r="AA3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AB3" s="7" t="n">
+      <c r="AB3" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="AC3" s="7" t="n">
+      <c r="AC3" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="AD3" s="7" t="n">
+      <c r="AD3" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="AE3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AQ3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV3" s="23" t="s">
+      <c r="AE3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU3" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV3" s="24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="str">
+      <c r="A4" s="20" t="str">
         <f aca="false">INDEX(participants!A:A,MATCH(B4,participants!C:C,0))&amp;" "&amp;INDEX(participants!B:B,MATCH(B4,participants!C:C,0))</f>
         <v>Clark Kent</v>
       </c>
-      <c r="B4" s="19" t="n">
+      <c r="B4" s="20" t="n">
         <v>1234567</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="21" t="str">
+      <c r="E4" s="22" t="str">
         <f aca="false">IF(LEN( AE4)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF4)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG4)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH4)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI4)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ4)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK4)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL4)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM4)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN4)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO4)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP4)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ4)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR4)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS4)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT4)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU4)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU4&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV4)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV4&amp;CHAR(10),"")</f>
         <v>## 1.1
 Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat
@@ -1316,155 +1427,155 @@
 ## Presentation
 Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat</v>
       </c>
-      <c r="F4" s="22" t="n">
+      <c r="F4" s="23" t="n">
         <f aca="false">ROUND(K4/70*100,0)</f>
         <v>53</v>
       </c>
-      <c r="G4" s="22" t="n">
+      <c r="G4" s="23" t="n">
         <f aca="false">ROUND(SUM(M4:P4)/SUM(M$1:P$1)*100,0)</f>
         <v>37</v>
       </c>
-      <c r="H4" s="22" t="n">
+      <c r="H4" s="23" t="n">
         <f aca="false">ROUND(SUM(N4:Q4)/SUM(N$1:Q$1)*100,0)</f>
         <v>35</v>
       </c>
-      <c r="I4" s="22" t="n">
+      <c r="I4" s="23" t="n">
         <f aca="false">ROUND(SUM(O4:R4)/SUM(O$1:R$1)*100,0)</f>
         <v>36</v>
       </c>
-      <c r="J4" s="22" t="n">
+      <c r="J4" s="23" t="n">
         <f aca="false">ROUND(SUM(P4:S4)/SUM(P$1:S$1)*100,0)</f>
         <v>47</v>
       </c>
-      <c r="K4" s="22" t="n">
+      <c r="K4" s="23" t="n">
         <f aca="false">ROUNDUP(SUM(M4:AD4),0)</f>
         <v>37</v>
       </c>
-      <c r="L4" s="19"/>
-      <c r="M4" s="7" t="n">
+      <c r="L4" s="20"/>
+      <c r="M4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N4" s="7" t="n">
+      <c r="N4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="O4" s="7" t="n">
+      <c r="O4" s="8" t="n">
         <v>0.5</v>
       </c>
-      <c r="P4" s="7" t="n">
+      <c r="P4" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" s="7" t="n">
+      <c r="Q4" s="8" t="n">
         <v>3.5</v>
       </c>
-      <c r="R4" s="7" t="n">
+      <c r="R4" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="S4" s="7" t="n">
+      <c r="S4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="T4" s="7" t="n">
+      <c r="T4" s="8" t="n">
         <v>3.5</v>
       </c>
-      <c r="U4" s="7" t="n">
+      <c r="U4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="V4" s="7" t="n">
+      <c r="V4" s="8" t="n">
         <v>1.1</v>
       </c>
-      <c r="W4" s="7" t="n">
+      <c r="W4" s="8" t="n">
         <v>0.6</v>
       </c>
-      <c r="X4" s="7" t="n">
+      <c r="X4" s="8" t="n">
         <v>0.5</v>
       </c>
-      <c r="Y4" s="7" t="n">
+      <c r="Y4" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="Z4" s="7" t="n">
+      <c r="Z4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AA4" s="7" t="n">
+      <c r="AA4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AB4" s="7" t="n">
+      <c r="AB4" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="AC4" s="7" t="n">
+      <c r="AC4" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="AD4" s="7" t="n">
+      <c r="AD4" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="AE4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AQ4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU4" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV4" s="23" t="s">
+      <c r="AE4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV4" s="24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="19" t="str">
+      <c r="A5" s="20" t="str">
         <f aca="false">INDEX(participants!A:A,MATCH(B5,participants!C:C,0))&amp;" "&amp;INDEX(participants!B:B,MATCH(B5,participants!C:C,0))</f>
         <v>Diana Prince</v>
       </c>
-      <c r="B5" s="19" t="n">
+      <c r="B5" s="20" t="n">
         <v>1234568</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="21" t="str">
+      <c r="E5" s="22" t="str">
         <f aca="false">IF(LEN( AE5)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF5)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG5)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH5)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI5)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ5)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK5)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL5)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM5)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN5)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO5)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP5)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ5)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR5)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS5)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT5)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU5)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU5&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV5)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV5&amp;CHAR(10),"")</f>
         <v>## 1.1
 Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat
@@ -1503,142 +1614,142 @@
 ## Presentation
 Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat</v>
       </c>
-      <c r="F5" s="22" t="n">
+      <c r="F5" s="23" t="n">
         <f aca="false">ROUND(K5/70*100,0)</f>
         <v>67</v>
       </c>
-      <c r="G5" s="22" t="n">
+      <c r="G5" s="23" t="n">
         <f aca="false">ROUND(SUM(M5:P5)/SUM(M$1:P$1)*100,0)</f>
         <v>50</v>
       </c>
-      <c r="H5" s="22" t="n">
+      <c r="H5" s="23" t="n">
         <f aca="false">ROUND(SUM(N5:Q5)/SUM(N$1:Q$1)*100,0)</f>
         <v>50</v>
       </c>
-      <c r="I5" s="22" t="n">
+      <c r="I5" s="23" t="n">
         <f aca="false">ROUND(SUM(O5:R5)/SUM(O$1:R$1)*100,0)</f>
         <v>43</v>
       </c>
-      <c r="J5" s="22" t="n">
+      <c r="J5" s="23" t="n">
         <f aca="false">ROUND(SUM(P5:S5)/SUM(P$1:S$1)*100,0)</f>
         <v>63</v>
       </c>
-      <c r="K5" s="22" t="n">
+      <c r="K5" s="23" t="n">
         <f aca="false">ROUNDUP(SUM(M5:AD5),0)</f>
         <v>47</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="7" t="n">
+      <c r="L5" s="21"/>
+      <c r="M5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N5" s="7" t="n">
+      <c r="N5" s="8" t="n">
         <v>4.5</v>
       </c>
-      <c r="O5" s="7" t="n">
+      <c r="O5" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="P5" s="7" t="n">
+      <c r="P5" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" s="7" t="n">
+      <c r="Q5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="R5" s="7" t="n">
+      <c r="R5" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="S5" s="7" t="n">
+      <c r="S5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="T5" s="7" t="n">
+      <c r="T5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="U5" s="7" t="n">
+      <c r="U5" s="8" t="n">
         <v>3.5</v>
       </c>
-      <c r="V5" s="7" t="n">
+      <c r="V5" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="W5" s="7" t="n">
+      <c r="W5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="X5" s="7" t="n">
+      <c r="X5" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Y5" s="7" t="n">
+      <c r="Y5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="Z5" s="7" t="n">
+      <c r="Z5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="AA5" s="7" t="n">
+      <c r="AA5" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="AB5" s="7" t="n">
+      <c r="AB5" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="AC5" s="7" t="n">
+      <c r="AC5" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="AD5" s="7" t="n">
+      <c r="AD5" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="AE5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AP5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AQ5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AR5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV5" s="23" t="s">
+      <c r="AE5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV5" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="str">
+    <row r="6" customFormat="false" ht="32.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="str">
         <f aca="false">INDEX(participants!A:A,MATCH(B6,participants!C:C,0))&amp;" "&amp;INDEX(participants!B:B,MATCH(B6,participants!C:C,0))</f>
         <v>Barry Alan</v>
       </c>
@@ -1648,36 +1759,36 @@
       <c r="C6" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="21" t="str">
+      <c r="D6" s="20"/>
+      <c r="E6" s="22" t="str">
         <f aca="false">IF(LEN( AE6)&gt;2,"## "&amp; AE$2&amp;CHAR(10)&amp;CHAR(10)&amp; AE6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AF6)&gt;2,"## "&amp;AF$2&amp;CHAR(10)&amp;CHAR(10)&amp;AF6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AG6)&gt;2,"## "&amp;AG$2&amp;CHAR(10)&amp;CHAR(10)&amp;AG6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AH6)&gt;2,"## "&amp;AH$2&amp;CHAR(10)&amp;CHAR(10)&amp;AH6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AI6)&gt;2,"## "&amp;AI$2&amp;CHAR(10)&amp;CHAR(10)&amp;AI6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AJ6)&gt;2,"## "&amp;AJ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AJ6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AK6)&gt;2,"## "&amp;AK$2&amp;CHAR(10)&amp;CHAR(10)&amp;AK6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AL6)&gt;2,"## "&amp;AL$2&amp;CHAR(10)&amp;CHAR(10)&amp;AL6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AM6)&gt;2,"## "&amp;AM$2&amp;CHAR(10)&amp;CHAR(10)&amp;AM6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AN6)&gt;2,"## "&amp;AN$2&amp;CHAR(10)&amp;CHAR(10)&amp;AN6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AO6)&gt;2,"## "&amp;AO$2&amp;CHAR(10)&amp;CHAR(10)&amp;AO6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AP6)&gt;2,"## "&amp;AP$2&amp;CHAR(10)&amp;CHAR(10)&amp;AP6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AQ6)&gt;2,"## "&amp;AQ$2&amp;CHAR(10)&amp;CHAR(10)&amp;AQ6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AR6)&gt;2,"## "&amp;AR$2&amp;CHAR(10)&amp;CHAR(10)&amp;AR6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AS6)&gt;2,"## "&amp;AS$2&amp;CHAR(10)&amp;CHAR(10)&amp;AS6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AT6)&gt;2,"## "&amp;AT$2&amp;CHAR(10)&amp;CHAR(10)&amp;AT6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AU6)&gt;2,"## "&amp;AU$2&amp;CHAR(10)&amp;CHAR(10)&amp;AU6&amp;CHAR(10)&amp;CHAR(10)&amp;CHAR(10),"")&amp;  IF(LEN(AV6)&gt;2,"## "&amp;AV$2&amp;CHAR(10)&amp;CHAR(10)&amp;AV6&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="F6" s="22" t="n">
+      <c r="F6" s="23" t="n">
         <f aca="false">ROUND(K6/70*100,0)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="22" t="n">
+      <c r="G6" s="23" t="n">
         <f aca="false">ROUND(SUM(M6:P6)/SUM(M$1:P$1)*100,0)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="22" t="n">
+      <c r="H6" s="23" t="n">
         <f aca="false">ROUND(SUM(N6:Q6)/SUM(N$1:Q$1)*100,0)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="22" t="n">
+      <c r="I6" s="23" t="n">
         <f aca="false">ROUND(SUM(O6:R6)/SUM(O$1:R$1)*100,0)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="22" t="n">
+      <c r="J6" s="23" t="n">
         <f aca="false">ROUND(SUM(P6:S6)/SUM(P$1:S$1)*100,0)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="22" t="n">
+      <c r="K6" s="23" t="n">
         <f aca="false">ROUNDUP(SUM(M6:AD6),0)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="19"/>
+      <c r="L6" s="20"/>
     </row>
     <row r="1048126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048127" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>